<commit_message>
fix(Opportunity): Mapped HW/SW Country Codes
* Mapped Hardware & Software Country Codes to the corresponding Addresses while Importing Opportunities
</commit_message>
<xml_diff>
--- a/tests/Feature/Data/opportunity/accounts-23032022.xlsx
+++ b/tests/Feature/Data/opportunity/accounts-23032022.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t>CH</t>
   </si>
   <si>
     <t>urs.gygax@ch.abb.com</t>
@@ -188,7 +191,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color indexed="64"/>
       <sz val="9.000000"/>
     </font>
     <font>
@@ -745,7 +747,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView topLeftCell="I1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -991,27 +993,27 @@
         <v>43</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>0</v>
@@ -1021,13 +1023,13 @@
         <v>0</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pipeliner Integration - Level 2 - init
</commit_message>
<xml_diff>
--- a/tests/Feature/Data/opportunity/accounts-23032022.xlsx
+++ b/tests/Feature/Data/opportunity/accounts-23032022.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t>CH</t>
   </si>
   <si>
     <t>urs.gygax@ch.abb.com</t>
@@ -191,6 +188,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <color indexed="64"/>
       <sz val="9.000000"/>
     </font>
     <font>
@@ -747,7 +745,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0" zoomScale="100">
+    <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -993,27 +991,27 @@
         <v>43</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>0</v>
@@ -1023,13 +1021,13 @@
         <v>0</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>